<commit_message>
Updated GDD's movement section and audience section. Task Schedule has also been touched up
</commit_message>
<xml_diff>
--- a/GameDesign/TaskScheduleGDD.xlsx
+++ b/GameDesign/TaskScheduleGDD.xlsx
@@ -1,18 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAFri\Documents\Unity Repos\Mecha-Crusades-Repo\GameDesign\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395D1C1E-968D-4691-95AB-88743C79A9AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -21,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>Today's Date:</t>
   </si>
@@ -144,15 +158,15 @@
     <t>Schedule &amp; Tasks</t>
   </si>
   <si>
-    <t>John Doe</t>
+    <t>Leo Frilot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -488,23 +502,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -517,22 +520,11 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
       <protection locked="0"/>
@@ -545,90 +537,143 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="11" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -772,6 +817,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1063,26 +1111,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BW48"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="33" customWidth="1"/>
+    <col min="3" max="3" width="9" style="43" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="43" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" customHeight="1">
+    <row r="1" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>39</v>
       </c>
@@ -1091,454 +1139,480 @@
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
     </row>
-    <row r="2" spans="1:5" ht="14" hidden="1" customHeight="1">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-    </row>
-    <row r="3" spans="1:5" hidden="1">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-    </row>
-    <row r="4" spans="1:5" ht="14" hidden="1" customHeight="1">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="17" t="s">
+    <row r="2" spans="1:5" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-    </row>
-    <row r="6" spans="1:5" hidden="1">
-      <c r="A6" s="17" t="s">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="19"/>
-    </row>
-    <row r="7" spans="1:5" hidden="1">
-      <c r="A7" s="17" t="s">
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="24">
         <v>41717</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="18" t="str">
+      <c r="C7" s="24"/>
+      <c r="D7" s="44" t="str">
         <f>TEXT(B7,"dddd")</f>
         <v>Wednesday</v>
       </c>
-      <c r="E7" s="19"/>
-    </row>
-    <row r="8" spans="1:5" hidden="1">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="19"/>
-    </row>
-    <row r="9" spans="1:5" ht="64.5" customHeight="1">
-      <c r="A9" s="23" t="s">
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="28" customFormat="1">
-      <c r="A10" s="24" t="s">
+    <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="32"/>
-    </row>
-    <row r="11" spans="1:5" s="28" customFormat="1">
-      <c r="A11" s="25" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="19"/>
+    </row>
+    <row r="11" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="36"/>
-    </row>
-    <row r="12" spans="1:5" s="28" customFormat="1">
-      <c r="A12" s="26" t="s">
+      <c r="B11" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="36"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="20"/>
+    </row>
+    <row r="12" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="34">
-        <v>42262</v>
-      </c>
-      <c r="D12" s="35">
-        <v>42267</v>
-      </c>
-      <c r="E12" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="28" customFormat="1">
-      <c r="A13" s="26" t="s">
+      <c r="C12" s="36"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="20"/>
+    </row>
+    <row r="13" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="36"/>
-    </row>
-    <row r="14" spans="1:5" s="28" customFormat="1">
-      <c r="A14" s="25" t="s">
+      <c r="B13" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="36">
+        <v>43982</v>
+      </c>
+      <c r="D13" s="46"/>
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="36"/>
-    </row>
-    <row r="15" spans="1:5" s="28" customFormat="1">
-      <c r="A15" s="26" t="s">
+      <c r="B14" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="36"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="20"/>
+    </row>
+    <row r="15" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
-    </row>
-    <row r="16" spans="1:5" s="28" customFormat="1">
-      <c r="A16" s="26" t="s">
+      <c r="B15" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="36"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="20"/>
+    </row>
+    <row r="16" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="36"/>
-    </row>
-    <row r="17" spans="1:5" s="28" customFormat="1">
-      <c r="A17" s="26" t="s">
+      <c r="B16" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="36"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="20"/>
+    </row>
+    <row r="17" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="36"/>
-    </row>
-    <row r="18" spans="1:5" s="28" customFormat="1">
-      <c r="A18" s="25" t="s">
+      <c r="B17" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="36"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="36"/>
-    </row>
-    <row r="19" spans="1:5" s="28" customFormat="1">
-      <c r="A19" s="26" t="s">
+      <c r="B18" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="36"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="20"/>
+    </row>
+    <row r="19" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="36"/>
-    </row>
-    <row r="20" spans="1:5" s="28" customFormat="1">
-      <c r="A20" s="26" t="s">
+      <c r="B19" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="36"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="20"/>
+    </row>
+    <row r="20" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="36"/>
-    </row>
-    <row r="21" spans="1:5" s="28" customFormat="1">
-      <c r="A21" s="26" t="s">
+      <c r="B20" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="36"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="20"/>
+    </row>
+    <row r="21" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="36"/>
-    </row>
-    <row r="22" spans="1:5" s="28" customFormat="1">
-      <c r="A22" s="26" t="s">
+      <c r="B21" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="36"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="20"/>
+    </row>
+    <row r="22" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="36"/>
-    </row>
-    <row r="23" spans="1:5" s="28" customFormat="1">
-      <c r="A23" s="25" t="s">
+      <c r="B22" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="36"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="20"/>
+    </row>
+    <row r="23" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="36"/>
-    </row>
-    <row r="24" spans="1:5" s="28" customFormat="1">
-      <c r="A24" s="26" t="s">
+      <c r="B23" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="36"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="20"/>
+    </row>
+    <row r="24" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="36"/>
-    </row>
-    <row r="25" spans="1:5" s="28" customFormat="1">
-      <c r="A25" s="26" t="s">
+      <c r="B24" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="36"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="20"/>
+    </row>
+    <row r="25" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="36"/>
-    </row>
-    <row r="26" spans="1:5" s="28" customFormat="1">
-      <c r="A26" s="25" t="s">
+      <c r="B25" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="36"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="20"/>
+    </row>
+    <row r="26" spans="1:5" s="18" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="36"/>
-    </row>
-    <row r="27" spans="1:5" s="28" customFormat="1">
-      <c r="A27" s="24" t="s">
+      <c r="B26" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="36"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="20"/>
+    </row>
+    <row r="27" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="32"/>
-    </row>
-    <row r="28" spans="1:5" s="28" customFormat="1">
-      <c r="A28" s="25" t="s">
+      <c r="B27" s="26"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="19"/>
+    </row>
+    <row r="28" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="36"/>
-    </row>
-    <row r="29" spans="1:5" s="28" customFormat="1">
-      <c r="A29" s="25" t="s">
+      <c r="B28" s="27"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="20"/>
+    </row>
+    <row r="29" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="36"/>
-    </row>
-    <row r="30" spans="1:5" s="28" customFormat="1">
-      <c r="A30" s="25" t="s">
+      <c r="B29" s="27"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="20"/>
+    </row>
+    <row r="30" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="36"/>
-    </row>
-    <row r="31" spans="1:5" s="28" customFormat="1" ht="28">
-      <c r="A31" s="25" t="s">
+      <c r="B30" s="27"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="20"/>
+    </row>
+    <row r="31" spans="1:5" s="18" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="36"/>
-    </row>
-    <row r="32" spans="1:5" s="28" customFormat="1">
-      <c r="A32" s="24" t="s">
+      <c r="B31" s="27"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="20"/>
+    </row>
+    <row r="32" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="29"/>
+      <c r="B32" s="26"/>
       <c r="C32" s="37"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="32"/>
-    </row>
-    <row r="33" spans="1:5" s="28" customFormat="1">
-      <c r="A33" s="25" t="s">
+      <c r="D32" s="47"/>
+      <c r="E32" s="19"/>
+    </row>
+    <row r="33" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="36"/>
-    </row>
-    <row r="34" spans="1:5" s="28" customFormat="1">
-      <c r="A34" s="25" t="s">
+      <c r="B33" s="27"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="20"/>
+    </row>
+    <row r="34" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="33"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="36"/>
-    </row>
-    <row r="35" spans="1:5" s="28" customFormat="1">
-      <c r="A35" s="27" t="s">
+      <c r="B34" s="27"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="39"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="42"/>
-    </row>
-    <row r="36" spans="1:5" hidden="1">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-    </row>
-    <row r="37" spans="1:5" hidden="1">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-    </row>
-    <row r="38" spans="1:5" hidden="1">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-    </row>
-    <row r="39" spans="1:5" hidden="1">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-    </row>
-    <row r="40" spans="1:5" hidden="1">
-      <c r="A40" s="7" t="s">
+      <c r="B35" s="28"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="21"/>
+    </row>
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="11">
+      <c r="B40" s="30"/>
+      <c r="C40" s="40">
         <v>39818</v>
       </c>
-      <c r="D40" s="12" t="e">
+      <c r="D40" s="49" t="e">
         <f>C40+#REF!-1</f>
         <v>#REF!</v>
       </c>
-      <c r="E40" s="9" t="e">
+      <c r="E40" s="5" t="e">
         <f>SUMPRODUCT(#REF!,E41:E43)/SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="3">
+      <c r="B41" s="31"/>
+      <c r="C41" s="41">
         <v>39818</v>
       </c>
-      <c r="D41" s="4" t="e">
+      <c r="D41" s="50" t="e">
         <f>C41+#REF!-1</f>
         <v>#REF!</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E41" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1">
-      <c r="A42" s="6" t="s">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="3">
+      <c r="B42" s="31"/>
+      <c r="C42" s="41">
         <v>39818</v>
       </c>
-      <c r="D42" s="4" t="e">
+      <c r="D42" s="50" t="e">
         <f>C42+#REF!-1</f>
         <v>#REF!</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E42" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1">
-      <c r="A43" s="13" t="s">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="3">
+      <c r="B43" s="31"/>
+      <c r="C43" s="41">
         <v>39818</v>
       </c>
-      <c r="D43" s="4" t="e">
+      <c r="D43" s="50" t="e">
         <f>C43+#REF!-1</f>
         <v>#REF!</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="14"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="14"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="14"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="8"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="8"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="8"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="8"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="42"/>
+      <c r="D47" s="42"/>
+      <c r="E47" s="8"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="8"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1557,12 +1631,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1574,12 +1648,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>